<commit_message>
update final entrega 3
</commit_message>
<xml_diff>
--- a/Documentação/Relatório de atividades Final.xlsx
+++ b/Documentação/Relatório de atividades Final.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Projeto_PHP\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E71138D-7620-410E-B08E-147B09D6E91A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="570" windowWidth="19815" windowHeight="7875"/>
+    <workbookView xWindow="390" yWindow="570" windowWidth="19815" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Página1" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
   <si>
     <t>Alunos</t>
   </si>
@@ -97,13 +98,28 @@
   </si>
   <si>
     <t>Justificativa do uso da arquitetura, tecnologias e padrões</t>
+  </si>
+  <si>
+    <t>Rafael, Willian, Gabriel</t>
+  </si>
+  <si>
+    <t>Estudo de uma estratégia para o modelo</t>
+  </si>
+  <si>
+    <t>Modelagem das tabelas financeiras</t>
+  </si>
+  <si>
+    <t>Criação do modelo inicial</t>
+  </si>
+  <si>
+    <t>Revisão, correção e complementação</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -121,13 +137,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -160,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -168,7 +177,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -198,7 +206,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -217,7 +225,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -255,7 +263,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -290,6 +298,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -325,9 +350,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -500,14 +542,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:C15"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -672,7 +714,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -680,6 +722,50 @@
       </c>
       <c r="C15" s="5" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>